<commit_message>
biorxiv version data updated.
</commit_message>
<xml_diff>
--- a/examples/input/models/ModelB_boolean_biorecipe.xlsx
+++ b/examples/input/models/ModelB_boolean_biorecipe.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasmine/Desktop/violin_reading/examples/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasmine/Desktop/github_local_copy/VIOLIN/examples/input/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F221B66-0C33-6842-98E6-D2836CB3F21A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518C42C8-D802-D543-AFE9-38EB53418126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5960" yWindow="3640" windowWidth="25220" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -466,9 +466,6 @@
     <t>TCR_LOW,TCR_HIGH</t>
   </si>
   <si>
-    <t>Element sub-type</t>
-  </si>
-  <si>
     <t>(FOS,JUN)</t>
   </si>
   <si>
@@ -509,6 +506,9 @@
   </si>
   <si>
     <t>I</t>
+  </si>
+  <si>
+    <t>Element Subtype</t>
   </si>
 </sst>
 </file>
@@ -1352,7 +1352,7 @@
   <dimension ref="A1:AP49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="O39" sqref="O39"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1379,7 +1379,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="E1" t="s">
         <v>32</v>
@@ -1507,10 +1507,10 @@
         <v>105</v>
       </c>
       <c r="O2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="S2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Z2" t="s">
         <v>135</v>
@@ -1547,10 +1547,10 @@
         <v>9</v>
       </c>
       <c r="O4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Z4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AB4" t="s">
         <v>8</v>
@@ -1564,7 +1564,7 @@
         <v>15</v>
       </c>
       <c r="O5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Z5" t="s">
         <v>95</v>
@@ -1612,7 +1612,7 @@
         <v>108</v>
       </c>
       <c r="O8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Z8" t="s">
         <v>136</v>
@@ -1646,7 +1646,7 @@
         <v>110</v>
       </c>
       <c r="O10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Z10" t="s">
         <v>78</v>
@@ -1666,7 +1666,7 @@
         <v>14</v>
       </c>
       <c r="O11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Z11" t="s">
         <v>12</v>
@@ -1686,13 +1686,13 @@
         <v>111</v>
       </c>
       <c r="O12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="S12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="Z12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AA12" t="s">
         <v>80</v>
@@ -1712,13 +1712,13 @@
         <v>112</v>
       </c>
       <c r="O13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="S13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="Z13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AA13" t="s">
         <v>73</v>
@@ -1738,7 +1738,7 @@
         <v>112</v>
       </c>
       <c r="O14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Z14" t="s">
         <v>137</v>
@@ -1761,7 +1761,7 @@
         <v>113</v>
       </c>
       <c r="O15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Z15" t="s">
         <v>138</v>
@@ -1781,7 +1781,7 @@
         <v>30</v>
       </c>
       <c r="O16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Z16" t="s">
         <v>139</v>
@@ -1804,7 +1804,7 @@
         <v>114</v>
       </c>
       <c r="O17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Z17" t="s">
         <v>79</v>
@@ -1824,7 +1824,7 @@
         <v>115</v>
       </c>
       <c r="O18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Z18" t="s">
         <v>16</v>
@@ -1844,7 +1844,7 @@
         <v>116</v>
       </c>
       <c r="O19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Z19" t="s">
         <v>24</v>
@@ -1864,7 +1864,7 @@
         <v>117</v>
       </c>
       <c r="O20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Z20" t="s">
         <v>94</v>
@@ -1884,10 +1884,10 @@
         <v>118</v>
       </c>
       <c r="O21" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Z21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AB21" t="s">
         <v>80</v>
@@ -1907,10 +1907,10 @@
         <v>119</v>
       </c>
       <c r="O22" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S22" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Z22" t="s">
         <v>91</v>
@@ -1950,13 +1950,13 @@
         <v>120</v>
       </c>
       <c r="O24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="S24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Z24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA24" t="s">
         <v>92</v>
@@ -1976,10 +1976,10 @@
         <v>121</v>
       </c>
       <c r="O25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Z25" t="s">
         <v>68</v>
@@ -2019,7 +2019,7 @@
         <v>122</v>
       </c>
       <c r="O27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Z27" t="s">
         <v>140</v>
@@ -2039,7 +2039,7 @@
         <v>123</v>
       </c>
       <c r="O28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Z28" t="s">
         <v>20</v>
@@ -2059,7 +2059,7 @@
         <v>124</v>
       </c>
       <c r="O29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Z29" t="s">
         <v>141</v>
@@ -2079,7 +2079,7 @@
         <v>124</v>
       </c>
       <c r="O30" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="Z30" t="s">
         <v>142</v>
@@ -2099,7 +2099,7 @@
         <v>124</v>
       </c>
       <c r="O31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="Z31" t="s">
         <v>143</v>
@@ -2136,10 +2136,10 @@
         <v>21</v>
       </c>
       <c r="O33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Z33" t="s">
         <v>85</v>
@@ -2162,10 +2162,10 @@
         <v>21</v>
       </c>
       <c r="O34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Z34" t="s">
         <v>86</v>
@@ -2188,7 +2188,7 @@
         <v>125</v>
       </c>
       <c r="O35" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Z35" t="s">
         <v>145</v>
@@ -2208,7 +2208,7 @@
         <v>28</v>
       </c>
       <c r="O36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Z36" t="s">
         <v>92</v>
@@ -2228,13 +2228,13 @@
         <v>23</v>
       </c>
       <c r="O37" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="S37" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="Z37" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AA37" t="s">
         <v>96</v>
@@ -2254,7 +2254,7 @@
         <v>126</v>
       </c>
       <c r="O38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Z38" t="s">
         <v>25</v>
@@ -2274,7 +2274,7 @@
         <v>127</v>
       </c>
       <c r="O39" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="Z39" t="s">
         <v>146</v>
@@ -2294,7 +2294,7 @@
         <v>128</v>
       </c>
       <c r="S40" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AA40" t="s">
         <v>99</v>
@@ -2314,7 +2314,7 @@
         <v>129</v>
       </c>
       <c r="O41" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Z41" t="s">
         <v>17</v>
@@ -2334,7 +2334,7 @@
         <v>130</v>
       </c>
       <c r="O42" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Z42" t="s">
         <v>98</v>
@@ -2354,7 +2354,7 @@
         <v>131</v>
       </c>
       <c r="O43" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Z43" t="s">
         <v>29</v>
@@ -2374,7 +2374,7 @@
         <v>132</v>
       </c>
       <c r="O44" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Z44" t="s">
         <v>89</v>
@@ -2394,7 +2394,7 @@
         <v>133</v>
       </c>
       <c r="O45" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Z45" t="s">
         <v>147</v>
@@ -2456,7 +2456,7 @@
         <v>134</v>
       </c>
       <c r="S49" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AA49" t="s">
         <v>7</v>

</xml_diff>